<commit_message>
Untested controller FSM code
</commit_message>
<xml_diff>
--- a/Final/PA3 pt1/Description and Sketches/NSPS Diagram.xlsx
+++ b/Final/PA3 pt1/Description and Sketches/NSPS Diagram.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/GDrive/Documents/School/3.Harvard/6.Junior Spring 2019/CS141 - Computer Architecture/cs141_Spring19/Final/PA3 pt1/Description and Sketches/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Billy/Virtual Machines/Shared files/Final/PA3 pt1/Description and Sketches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1B61F8-62E9-2741-B488-96DC41E2C3C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6279D65C-E70D-7E49-B987-6AF2C2D983A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{F516D808-5618-2F49-B3A1-E5FF1118C11B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" xr2:uid="{F516D808-5618-2F49-B3A1-E5FF1118C11B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
   <si>
     <t>State</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>4'b1010 (10)</t>
+  </si>
+  <si>
+    <t>NSEW_Flag</t>
+  </si>
+  <si>
+    <t>NSRED</t>
+  </si>
+  <si>
+    <t>EWRED</t>
   </si>
 </sst>
 </file>
@@ -556,109 +565,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -980,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB341713-1585-AE43-BBEA-C8ADEBA4DA5A}">
-  <dimension ref="A1:AK22"/>
+  <dimension ref="A1:AK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1001,159 +1010,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="32" t="s">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="44" t="s">
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="46"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="48"/>
     </row>
     <row r="2" spans="1:37" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="41" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="47" t="s">
+      <c r="J2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="L2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="49" t="s">
+      <c r="O2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="48" t="s">
+      <c r="Q2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="48" t="s">
+      <c r="R2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="48" t="s">
+      <c r="S2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="48" t="s">
+      <c r="T2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="50" t="s">
+      <c r="U2" s="34" t="s">
         <v>28</v>
       </c>
+      <c r="V2" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="3" spans="1:37" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:37" s="24" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="26">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="27">
+      <c r="B3" s="24">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="25">
         <v>7</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="25">
-        <v>0</v>
-      </c>
-      <c r="K3" s="26">
-        <v>0</v>
-      </c>
-      <c r="L3" s="26">
-        <v>1</v>
-      </c>
-      <c r="M3" s="26">
-        <v>0</v>
-      </c>
-      <c r="N3" s="26">
-        <v>0</v>
-      </c>
-      <c r="O3" s="26">
-        <v>1</v>
-      </c>
-      <c r="P3" s="26">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="26">
-        <v>0</v>
-      </c>
-      <c r="R3" s="26">
-        <v>0</v>
-      </c>
-      <c r="S3" s="26">
-        <v>0</v>
-      </c>
-      <c r="T3" s="26">
-        <v>0</v>
-      </c>
-      <c r="U3" s="27">
+      <c r="E3" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="23">
+        <v>0</v>
+      </c>
+      <c r="K3" s="24">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24">
+        <v>1</v>
+      </c>
+      <c r="M3" s="24">
+        <v>0</v>
+      </c>
+      <c r="N3" s="24">
+        <v>0</v>
+      </c>
+      <c r="O3" s="24">
+        <v>1</v>
+      </c>
+      <c r="P3" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="24">
+        <v>0</v>
+      </c>
+      <c r="R3" s="24">
+        <v>0</v>
+      </c>
+      <c r="S3" s="24">
+        <v>0</v>
+      </c>
+      <c r="T3" s="24">
+        <v>0</v>
+      </c>
+      <c r="U3" s="25">
         <v>0</v>
       </c>
       <c r="V3" s="2"/>
@@ -1173,68 +1185,68 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:37" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:37" s="24" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="24">
         <v>7</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="27">
+      <c r="C4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="25">
         <v>2</v>
       </c>
-      <c r="E4" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="25">
-        <v>0</v>
-      </c>
-      <c r="K4" s="26">
-        <v>0</v>
-      </c>
-      <c r="L4" s="26">
-        <v>1</v>
-      </c>
-      <c r="M4" s="26">
-        <v>0</v>
-      </c>
-      <c r="N4" s="26">
-        <v>0</v>
-      </c>
-      <c r="O4" s="26">
-        <v>1</v>
-      </c>
-      <c r="P4" s="26">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="26">
-        <v>0</v>
-      </c>
-      <c r="R4" s="26">
-        <v>1</v>
-      </c>
-      <c r="S4" s="26">
-        <v>0</v>
-      </c>
-      <c r="T4" s="26">
-        <v>0</v>
-      </c>
-      <c r="U4" s="27">
+      <c r="E4" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="23">
+        <v>0</v>
+      </c>
+      <c r="K4" s="24">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
+        <v>1</v>
+      </c>
+      <c r="M4" s="24">
+        <v>0</v>
+      </c>
+      <c r="N4" s="24">
+        <v>0</v>
+      </c>
+      <c r="O4" s="24">
+        <v>1</v>
+      </c>
+      <c r="P4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="24">
+        <v>0</v>
+      </c>
+      <c r="R4" s="24">
+        <v>1</v>
+      </c>
+      <c r="S4" s="24">
+        <v>0</v>
+      </c>
+      <c r="T4" s="24">
+        <v>0</v>
+      </c>
+      <c r="U4" s="25">
         <v>0</v>
       </c>
       <c r="V4" s="2"/>
@@ -1344,7 +1356,7 @@
       <c r="D6" s="14">
         <v>9</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="22">
         <v>0</v>
       </c>
       <c r="F6" s="2">
@@ -1356,11 +1368,11 @@
       <c r="H6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="24"/>
-      <c r="U6" s="20"/>
+      <c r="I6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="22"/>
+      <c r="U6" s="18"/>
     </row>
     <row r="7" spans="1:37" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
@@ -1371,21 +1383,21 @@
       <c r="D7" s="14">
         <v>8</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="50"/>
       <c r="G7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="20">
-        <v>1</v>
-      </c>
-      <c r="J7" s="24"/>
-      <c r="U7" s="20"/>
+      <c r="I7" s="18">
+        <v>1</v>
+      </c>
+      <c r="J7" s="22"/>
+      <c r="U7" s="18"/>
     </row>
     <row r="8" spans="1:37" s="5" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -1396,10 +1408,10 @@
       <c r="D8" s="17">
         <v>9</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="29"/>
+      <c r="F8" s="52"/>
       <c r="G8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1428,65 +1440,65 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:37" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:37" s="24" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>8</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="25">
         <v>3</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="25">
-        <v>0</v>
-      </c>
-      <c r="K9" s="26">
-        <v>0</v>
-      </c>
-      <c r="L9" s="26">
-        <v>1</v>
-      </c>
-      <c r="M9" s="26">
-        <v>0</v>
-      </c>
-      <c r="N9" s="26">
-        <v>0</v>
-      </c>
-      <c r="O9" s="26">
-        <v>1</v>
-      </c>
-      <c r="P9" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="26">
-        <v>1</v>
-      </c>
-      <c r="R9" s="26">
-        <v>0</v>
-      </c>
-      <c r="S9" s="26">
-        <v>0</v>
-      </c>
-      <c r="T9" s="26" t="s">
+      <c r="E9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="23">
+        <v>0</v>
+      </c>
+      <c r="K9" s="24">
+        <v>0</v>
+      </c>
+      <c r="L9" s="24">
+        <v>1</v>
+      </c>
+      <c r="M9" s="24">
+        <v>0</v>
+      </c>
+      <c r="N9" s="24">
+        <v>0</v>
+      </c>
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
+      <c r="P9" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="24">
+        <v>1</v>
+      </c>
+      <c r="R9" s="24">
+        <v>0</v>
+      </c>
+      <c r="S9" s="24">
+        <v>0</v>
+      </c>
+      <c r="T9" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U9" s="27">
+      <c r="U9" s="25">
         <v>1</v>
       </c>
       <c r="V9" s="2"/>
@@ -1506,65 +1518,65 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:37" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:37" s="24" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="24">
         <v>9</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="25">
         <v>4</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="25">
-        <v>0</v>
-      </c>
-      <c r="K10" s="26">
-        <v>0</v>
-      </c>
-      <c r="L10" s="26">
-        <v>1</v>
-      </c>
-      <c r="M10" s="26">
-        <v>0</v>
-      </c>
-      <c r="N10" s="26">
-        <v>0</v>
-      </c>
-      <c r="O10" s="26">
-        <v>1</v>
-      </c>
-      <c r="P10" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="26">
-        <v>1</v>
-      </c>
-      <c r="R10" s="26">
-        <v>0</v>
-      </c>
-      <c r="S10" s="26">
-        <v>0</v>
-      </c>
-      <c r="T10" s="26" t="s">
+      <c r="E10" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="23">
+        <v>0</v>
+      </c>
+      <c r="K10" s="24">
+        <v>0</v>
+      </c>
+      <c r="L10" s="24">
+        <v>1</v>
+      </c>
+      <c r="M10" s="24">
+        <v>0</v>
+      </c>
+      <c r="N10" s="24">
+        <v>0</v>
+      </c>
+      <c r="O10" s="24">
+        <v>1</v>
+      </c>
+      <c r="P10" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="24">
+        <v>1</v>
+      </c>
+      <c r="R10" s="24">
+        <v>0</v>
+      </c>
+      <c r="S10" s="24">
+        <v>0</v>
+      </c>
+      <c r="T10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U10" s="27">
+      <c r="U10" s="25">
         <v>1</v>
       </c>
       <c r="V10" s="2"/>
@@ -1584,71 +1596,73 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:37" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:37" s="24" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="24">
         <v>3</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="24">
         <v>10</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="25">
         <v>10</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="26" t="s">
+      <c r="E11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="25">
-        <v>1</v>
-      </c>
-      <c r="K11" s="26">
-        <v>0</v>
-      </c>
-      <c r="L11" s="26">
-        <v>0</v>
-      </c>
-      <c r="M11" s="26">
-        <v>0</v>
-      </c>
-      <c r="N11" s="26">
-        <v>0</v>
-      </c>
-      <c r="O11" s="26">
-        <v>1</v>
-      </c>
-      <c r="P11" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="26">
-        <v>0</v>
-      </c>
-      <c r="R11" s="26">
-        <v>0</v>
-      </c>
-      <c r="S11" s="26">
-        <v>1</v>
-      </c>
-      <c r="T11" s="26" t="s">
+      <c r="I11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="23">
+        <v>1</v>
+      </c>
+      <c r="K11" s="24">
+        <v>0</v>
+      </c>
+      <c r="L11" s="24">
+        <v>0</v>
+      </c>
+      <c r="M11" s="24">
+        <v>0</v>
+      </c>
+      <c r="N11" s="24">
+        <v>0</v>
+      </c>
+      <c r="O11" s="24">
+        <v>1</v>
+      </c>
+      <c r="P11" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="24">
+        <v>0</v>
+      </c>
+      <c r="R11" s="24">
+        <v>0</v>
+      </c>
+      <c r="S11" s="24">
+        <v>1</v>
+      </c>
+      <c r="T11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U11" s="27">
-        <v>0</v>
-      </c>
-      <c r="V11" s="2"/>
+      <c r="U11" s="25">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -1665,68 +1679,70 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:37" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:37" s="24" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="24">
         <v>10</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="25">
         <v>5</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="25">
-        <v>1</v>
-      </c>
-      <c r="K12" s="26">
-        <v>0</v>
-      </c>
-      <c r="L12" s="26">
-        <v>0</v>
-      </c>
-      <c r="M12" s="26">
-        <v>0</v>
-      </c>
-      <c r="N12" s="26">
-        <v>0</v>
-      </c>
-      <c r="O12" s="26">
-        <v>1</v>
-      </c>
-      <c r="P12" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="26">
-        <v>0</v>
-      </c>
-      <c r="R12" s="26">
-        <v>0</v>
-      </c>
-      <c r="S12" s="26">
-        <v>0</v>
-      </c>
-      <c r="T12" s="26" t="s">
+      <c r="E12" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="23">
+        <v>1</v>
+      </c>
+      <c r="K12" s="24">
+        <v>0</v>
+      </c>
+      <c r="L12" s="24">
+        <v>0</v>
+      </c>
+      <c r="M12" s="24">
+        <v>0</v>
+      </c>
+      <c r="N12" s="24">
+        <v>0</v>
+      </c>
+      <c r="O12" s="24">
+        <v>1</v>
+      </c>
+      <c r="P12" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="24">
+        <v>0</v>
+      </c>
+      <c r="R12" s="24">
+        <v>0</v>
+      </c>
+      <c r="S12" s="24">
+        <v>0</v>
+      </c>
+      <c r="T12" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="U12" s="27">
-        <v>1</v>
-      </c>
-      <c r="V12" s="2"/>
+      <c r="U12" s="25">
+        <v>1</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -1743,71 +1759,73 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:37" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:37" s="24" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="24">
         <v>4</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="24">
         <v>10</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="25">
         <v>11</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="26" t="s">
+      <c r="E13" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="25">
-        <v>0</v>
-      </c>
-      <c r="K13" s="26">
-        <v>0</v>
-      </c>
-      <c r="L13" s="26">
-        <v>1</v>
-      </c>
-      <c r="M13" s="26">
-        <v>1</v>
-      </c>
-      <c r="N13" s="26">
-        <v>0</v>
-      </c>
-      <c r="O13" s="26">
-        <v>0</v>
-      </c>
-      <c r="P13" s="26">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="26">
-        <v>1</v>
-      </c>
-      <c r="R13" s="26">
-        <v>0</v>
-      </c>
-      <c r="S13" s="26">
-        <v>1</v>
-      </c>
-      <c r="T13" s="26" t="s">
+      <c r="I13" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="23">
+        <v>0</v>
+      </c>
+      <c r="K13" s="24">
+        <v>0</v>
+      </c>
+      <c r="L13" s="24">
+        <v>1</v>
+      </c>
+      <c r="M13" s="24">
+        <v>1</v>
+      </c>
+      <c r="N13" s="24">
+        <v>0</v>
+      </c>
+      <c r="O13" s="24">
+        <v>0</v>
+      </c>
+      <c r="P13" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>1</v>
+      </c>
+      <c r="R13" s="24">
+        <v>0</v>
+      </c>
+      <c r="S13" s="24">
+        <v>1</v>
+      </c>
+      <c r="T13" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="U13" s="27">
-        <v>0</v>
-      </c>
-      <c r="V13" s="2"/>
+      <c r="U13" s="25">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <v>1</v>
+      </c>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -1824,68 +1842,70 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:37" s="26" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:37" s="24" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="24">
         <v>11</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="25">
         <v>6</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="25">
-        <v>0</v>
-      </c>
-      <c r="K14" s="26">
-        <v>0</v>
-      </c>
-      <c r="L14" s="26">
-        <v>1</v>
-      </c>
-      <c r="M14" s="26">
-        <v>1</v>
-      </c>
-      <c r="N14" s="26">
-        <v>0</v>
-      </c>
-      <c r="O14" s="26">
-        <v>0</v>
-      </c>
-      <c r="P14" s="26">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="26">
-        <v>1</v>
-      </c>
-      <c r="R14" s="26">
-        <v>0</v>
-      </c>
-      <c r="S14" s="26">
-        <v>0</v>
-      </c>
-      <c r="T14" s="26" t="s">
+      <c r="E14" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="23">
+        <v>0</v>
+      </c>
+      <c r="K14" s="24">
+        <v>0</v>
+      </c>
+      <c r="L14" s="24">
+        <v>1</v>
+      </c>
+      <c r="M14" s="24">
+        <v>1</v>
+      </c>
+      <c r="N14" s="24">
+        <v>0</v>
+      </c>
+      <c r="O14" s="24">
+        <v>0</v>
+      </c>
+      <c r="P14" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="24">
+        <v>1</v>
+      </c>
+      <c r="R14" s="24">
+        <v>0</v>
+      </c>
+      <c r="S14" s="24">
+        <v>0</v>
+      </c>
+      <c r="T14" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="U14" s="27">
-        <v>1</v>
-      </c>
-      <c r="V14" s="2"/>
+      <c r="U14" s="25">
+        <v>1</v>
+      </c>
+      <c r="V14" s="2">
+        <v>1</v>
+      </c>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
@@ -1966,7 +1986,9 @@
       <c r="U15" s="11">
         <v>0</v>
       </c>
-      <c r="V15" s="2"/>
+      <c r="V15" s="2">
+        <v>0</v>
+      </c>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -2015,10 +2037,10 @@
       <c r="O16" s="16"/>
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="51"/>
-      <c r="T16" s="51"/>
-      <c r="U16" s="52"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="36"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
@@ -2036,72 +2058,75 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+    <row r="17" spans="1:22" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="20">
         <v>6</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="20">
         <v>5</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="21">
         <v>7</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="22">
-        <v>1</v>
-      </c>
-      <c r="H17" s="22" t="s">
+      <c r="E17" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="20">
+        <v>1</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="21">
-        <v>0</v>
-      </c>
-      <c r="K17" s="22">
-        <v>0</v>
-      </c>
-      <c r="L17" s="22">
-        <v>1</v>
-      </c>
-      <c r="M17" s="22">
-        <v>0</v>
-      </c>
-      <c r="N17" s="22">
-        <v>1</v>
-      </c>
-      <c r="O17" s="22">
-        <v>0</v>
-      </c>
-      <c r="P17" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="22">
-        <v>1</v>
-      </c>
-      <c r="R17" s="22">
-        <v>0</v>
-      </c>
-      <c r="S17" s="22">
-        <v>1</v>
-      </c>
-      <c r="T17" s="22" t="s">
+      <c r="I17" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="19">
+        <v>0</v>
+      </c>
+      <c r="K17" s="20">
+        <v>0</v>
+      </c>
+      <c r="L17" s="20">
+        <v>1</v>
+      </c>
+      <c r="M17" s="20">
+        <v>0</v>
+      </c>
+      <c r="N17" s="20">
+        <v>1</v>
+      </c>
+      <c r="O17" s="20">
+        <v>0</v>
+      </c>
+      <c r="P17" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>1</v>
+      </c>
+      <c r="R17" s="20">
+        <v>0</v>
+      </c>
+      <c r="S17" s="20">
+        <v>1</v>
+      </c>
+      <c r="T17" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="U17" s="23">
-        <v>0</v>
+      <c r="U17" s="21">
+        <v>0</v>
+      </c>
+      <c r="V17" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16">
@@ -2138,8 +2163,8 @@
       <c r="T18" s="16"/>
       <c r="U18" s="17"/>
     </row>
-    <row r="20" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F21" s="6" t="s">
         <v>30</v>
       </c>
@@ -2150,7 +2175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F22" s="4" t="s">
         <v>32</v>
       </c>
@@ -2159,17 +2184,25 @@
       </c>
       <c r="H22" s="7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="G23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:U1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added modified diagram to include 2bit NSEW_flag and added test bench for traffic controller
</commit_message>
<xml_diff>
--- a/Final/PA3 pt1/Description and Sketches/NSPS Diagram.xlsx
+++ b/Final/PA3 pt1/Description and Sketches/NSPS Diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Billy/Virtual Machines/Shared files/Final/PA3 pt1/Description and Sketches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6279D65C-E70D-7E49-B987-6AF2C2D983A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D81982B-0CA4-414C-B559-C8799427FBA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" xr2:uid="{F516D808-5618-2F49-B3A1-E5FF1118C11B}"/>
   </bookViews>
@@ -622,6 +622,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -656,18 +668,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -991,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB341713-1585-AE43-BBEA-C8ADEBA4DA5A}">
   <dimension ref="A1:AK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1010,45 +1010,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="39" t="s">
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="48"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="52"/>
     </row>
     <row r="2" spans="1:37" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="27"/>
-      <c r="D2" s="42"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="28" t="s">
         <v>5</v>
       </c>
@@ -1168,7 +1168,9 @@
       <c r="U3" s="25">
         <v>0</v>
       </c>
-      <c r="V3" s="2"/>
+      <c r="V3" s="2">
+        <v>10</v>
+      </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -1383,10 +1385,10 @@
       <c r="D7" s="14">
         <v>8</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="50"/>
+      <c r="F7" s="38"/>
       <c r="G7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1408,10 +1410,10 @@
       <c r="D8" s="17">
         <v>9</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="52"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="5" t="s">
         <v>18</v>
       </c>
@@ -2196,13 +2198,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="J1:U1"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>